<commit_message>
adding multi-variable linear regression result
</commit_message>
<xml_diff>
--- a/Resources/MLS_Historical_Performance.xlsx
+++ b/Resources/MLS_Historical_Performance.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BootCamp\Project1-WJBA\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C147086F-F608-4C56-A71A-C0CD99B6E9E4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9E359CC6-3F07-48AF-A986-A7E6150A42D1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" xr2:uid="{5AE5F6AD-B68E-4277-87A9-73AD4271E422}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Performance!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="31">
   <si>
     <t>New York Red Bulls</t>
   </si>
@@ -161,8 +164,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,22 +481,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFB8469-5EBE-4F44-B978-D01E4E8EFA51}">
-  <dimension ref="A1:H120"/>
+  <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
@@ -518,8 +523,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C2">
         <v>34</v>
@@ -528,24 +533,24 @@
         <v>19</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H2">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C3">
         <v>34</v>
@@ -563,275 +568,275 @@
         <v>63</v>
       </c>
       <c r="H3">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C4">
         <v>34</v>
       </c>
       <c r="D4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H4">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>0</v>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C5">
         <v>34</v>
       </c>
       <c r="D5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G5">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H5">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C6">
         <v>34</v>
       </c>
       <c r="D6">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G6">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H6">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C7">
         <v>34</v>
       </c>
       <c r="D7">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H7">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C8">
         <v>34</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F8">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G8">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H8">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>26</v>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C9">
         <v>34</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E9">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G9">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H9">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>1</v>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C10">
         <v>34</v>
       </c>
       <c r="D10">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F10">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G10">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H10">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C11">
         <v>34</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G11">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H11">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>30</v>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C12">
         <v>34</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E12">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F12">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G12">
         <v>43</v>
       </c>
       <c r="H12">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C13">
         <v>34</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G13">
         <v>42</v>
       </c>
       <c r="H13">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>15</v>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C14">
         <v>34</v>
@@ -849,160 +854,160 @@
         <v>39</v>
       </c>
       <c r="H14">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>16</v>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C15">
         <v>34</v>
       </c>
       <c r="D15">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E15">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G15">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H15">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>17</v>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C16">
         <v>34</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E16">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F16">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G16">
         <v>36</v>
       </c>
       <c r="H16">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>18</v>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C17">
         <v>34</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F17">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G17">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H17">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C18">
         <v>34</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E18">
         <v>16</v>
       </c>
       <c r="F18">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G18">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H18">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>20</v>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C19">
         <v>34</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19">
         <v>18</v>
       </c>
       <c r="F19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G19">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H19">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>34</v>
+      </c>
+      <c r="D20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20">
-        <v>34</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
       <c r="E20">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G20">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="H20">
         <v>2012</v>
@@ -1010,36 +1015,36 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C21">
         <v>34</v>
       </c>
       <c r="D21">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G21">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H21">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C22">
         <v>34</v>
@@ -1057,92 +1062,92 @@
         <v>58</v>
       </c>
       <c r="H22">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C23">
         <v>34</v>
       </c>
       <c r="D23">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F23">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G23">
         <v>57</v>
       </c>
       <c r="H23">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C24">
         <v>34</v>
       </c>
       <c r="D24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G24">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H24">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C25">
         <v>34</v>
       </c>
       <c r="D25">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E25">
         <v>11</v>
       </c>
       <c r="F25">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H25">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>6</v>
-      </c>
-      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C26">
@@ -1152,50 +1157,50 @@
         <v>15</v>
       </c>
       <c r="E26">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F26">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G26">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H26">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C27">
         <v>34</v>
       </c>
       <c r="D27">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E27">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F27">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G27">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H27">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>8</v>
-      </c>
-      <c r="B28" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C28">
         <v>34</v>
@@ -1204,299 +1209,299 @@
         <v>14</v>
       </c>
       <c r="E28">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F28">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G28">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H28">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>9</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C29">
         <v>34</v>
       </c>
       <c r="D29">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E29">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F29">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G29">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H29">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>10</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C30">
         <v>34</v>
       </c>
       <c r="D30">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E30">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F30">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G30">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H30">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>11</v>
-      </c>
-      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C31">
         <v>34</v>
       </c>
       <c r="D31">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E31">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F31">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G31">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H31">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>12</v>
-      </c>
-      <c r="B32" t="s">
-        <v>13</v>
+        <v>13</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C32">
         <v>34</v>
       </c>
       <c r="D32">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E32">
         <v>13</v>
       </c>
       <c r="F32">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G32">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H32">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>13</v>
-      </c>
-      <c r="B33" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C33">
         <v>34</v>
       </c>
       <c r="D33">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E33">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F33">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G33">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="H33">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>14</v>
-      </c>
-      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C34">
         <v>34</v>
       </c>
       <c r="D34">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E34">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F34">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G34">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H34">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>15</v>
-      </c>
-      <c r="B35" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
       <c r="D35">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E35">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F35">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G35">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="H35">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
+        <v>17</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36">
+        <v>34</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
         <v>16</v>
       </c>
-      <c r="B36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36">
-        <v>34</v>
-      </c>
-      <c r="D36">
-        <v>12</v>
-      </c>
-      <c r="E36">
-        <v>17</v>
-      </c>
       <c r="F36">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G36">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H36">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>17</v>
-      </c>
-      <c r="B37" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C37">
         <v>34</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E37">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F37">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G37">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H37">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>18</v>
-      </c>
-      <c r="B38" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C38">
         <v>34</v>
       </c>
       <c r="D38">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E38">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F38">
         <v>8</v>
       </c>
       <c r="G38">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H38">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>19</v>
-      </c>
-      <c r="B39" t="s">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C39">
         <v>34</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E39">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F39">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G39">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="H39">
         <v>2013</v>
@@ -1504,88 +1509,88 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C40">
         <v>34</v>
       </c>
       <c r="D40">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E40">
         <v>10</v>
       </c>
       <c r="F40">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G40">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H40">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>26</v>
+        <v>3</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C41">
         <v>34</v>
       </c>
       <c r="D41">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E41">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F41">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G41">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H41">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C42">
         <v>34</v>
       </c>
       <c r="D42">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E42">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F42">
         <v>8</v>
       </c>
       <c r="G42">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H42">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C43">
         <v>34</v>
@@ -1594,76 +1599,76 @@
         <v>15</v>
       </c>
       <c r="E43">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F43">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G43">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H43">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>5</v>
-      </c>
-      <c r="B44" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C44">
         <v>34</v>
       </c>
       <c r="D44">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E44">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F44">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G44">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H44">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>6</v>
-      </c>
-      <c r="B45" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C45">
         <v>34</v>
       </c>
       <c r="D45">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E45">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F45">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G45">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H45">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>7</v>
-      </c>
-      <c r="B46" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C46">
         <v>34</v>
@@ -1672,76 +1677,76 @@
         <v>14</v>
       </c>
       <c r="E46">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F46">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G46">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H46">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>8</v>
-      </c>
-      <c r="B47" t="s">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C47">
         <v>34</v>
       </c>
       <c r="D47">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E47">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F47">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G47">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H47">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>9</v>
-      </c>
-      <c r="B48" t="s">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C48">
         <v>34</v>
       </c>
       <c r="D48">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E48">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F48">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G48">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H48">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>10</v>
-      </c>
-      <c r="B49" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C49">
         <v>34</v>
@@ -1759,93 +1764,93 @@
         <v>49</v>
       </c>
       <c r="H49">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>11</v>
-      </c>
-      <c r="B50" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C50">
         <v>34</v>
       </c>
       <c r="D50">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E50">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F50">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G50">
         <v>49</v>
       </c>
       <c r="H50">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>12</v>
-      </c>
-      <c r="B51" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C51">
         <v>34</v>
       </c>
       <c r="D51">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E51">
         <v>12</v>
       </c>
       <c r="F51">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G51">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H51">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>13</v>
-      </c>
-      <c r="B52" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C52">
         <v>34</v>
       </c>
       <c r="D52">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E52">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F52">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H52">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C53">
         <v>34</v>
@@ -1854,143 +1859,143 @@
         <v>11</v>
       </c>
       <c r="E53">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F53">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G53">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H53">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>15</v>
-      </c>
-      <c r="B54" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C54">
         <v>34</v>
       </c>
       <c r="D54">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E54">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F54">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G54">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H54">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>16</v>
-      </c>
-      <c r="B55" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C55">
         <v>34</v>
       </c>
       <c r="D55">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E55">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F55">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G55">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H55">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>17</v>
-      </c>
-      <c r="B56" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C56">
         <v>34</v>
       </c>
       <c r="D56">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E56">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F56">
         <v>8</v>
       </c>
       <c r="G56">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H56">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>18</v>
-      </c>
-      <c r="B57" t="s">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C57">
         <v>34</v>
       </c>
       <c r="D57">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E57">
+        <v>24</v>
+      </c>
+      <c r="F57">
+        <v>7</v>
+      </c>
+      <c r="G57">
         <v>16</v>
       </c>
-      <c r="F57">
-        <v>12</v>
-      </c>
-      <c r="G57">
-        <v>30</v>
-      </c>
       <c r="H57">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>19</v>
-      </c>
-      <c r="B58" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C58">
         <v>34</v>
       </c>
       <c r="D58">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E58">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F58">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G58">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="H58">
         <v>2014</v>
@@ -1998,218 +2003,218 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>1</v>
-      </c>
-      <c r="B59" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C59">
         <v>34</v>
       </c>
       <c r="D59">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E59">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F59">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G59">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H59">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>2</v>
-      </c>
-      <c r="B60" t="s">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C60">
         <v>34</v>
       </c>
       <c r="D60">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E60">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G60">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H60">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>3</v>
-      </c>
-      <c r="B61" t="s">
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C61">
         <v>34</v>
       </c>
       <c r="D61">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E61">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F61">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G61">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H61">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62">
+        <v>34</v>
+      </c>
+      <c r="D62">
+        <v>17</v>
+      </c>
+      <c r="E62">
+        <v>13</v>
+      </c>
+      <c r="F62">
         <v>4</v>
       </c>
-      <c r="B62" t="s">
-        <v>14</v>
-      </c>
-      <c r="C62">
-        <v>34</v>
-      </c>
-      <c r="D62">
-        <v>15</v>
-      </c>
-      <c r="E62">
-        <v>11</v>
-      </c>
-      <c r="F62">
-        <v>8</v>
-      </c>
       <c r="G62">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H62">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>5</v>
-      </c>
-      <c r="B63" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C63">
         <v>34</v>
       </c>
       <c r="D63">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E63">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F63">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G63">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H63">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>6</v>
-      </c>
-      <c r="B64" t="s">
-        <v>29</v>
+        <v>7</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C64">
         <v>34</v>
       </c>
       <c r="D64">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E64">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F64">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G64">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H64">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>7</v>
-      </c>
-      <c r="B65" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C65">
         <v>34</v>
       </c>
       <c r="D65">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E65">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F65">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G65">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H65">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>8</v>
-      </c>
-      <c r="B66" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C66">
         <v>34</v>
       </c>
       <c r="D66">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E66">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F66">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G66">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H66">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>9</v>
-      </c>
-      <c r="B67" t="s">
-        <v>26</v>
+        <v>10</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C67">
         <v>34</v>
@@ -2218,273 +2223,273 @@
         <v>14</v>
       </c>
       <c r="E67">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F67">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G67">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H67">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>10</v>
-      </c>
-      <c r="B68" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C68">
         <v>34</v>
       </c>
       <c r="D68">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E68">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F68">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G68">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H68">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>11</v>
-      </c>
-      <c r="B69" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C69">
         <v>34</v>
       </c>
       <c r="D69">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E69">
         <v>12</v>
       </c>
       <c r="F69">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G69">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H69">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>12</v>
-      </c>
-      <c r="B70" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C70">
         <v>34</v>
       </c>
       <c r="D70">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E70">
         <v>15</v>
       </c>
       <c r="F70">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G70">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H70">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>13</v>
-      </c>
-      <c r="B71" t="s">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C71">
         <v>34</v>
       </c>
       <c r="D71">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E71">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F71">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G71">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H71">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>14</v>
-      </c>
-      <c r="B72" t="s">
-        <v>24</v>
+        <v>15</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C72">
         <v>34</v>
       </c>
       <c r="D72">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E72">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F72">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G72">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H72">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>15</v>
-      </c>
-      <c r="B73" t="s">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C73">
         <v>34</v>
       </c>
       <c r="D73">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E73">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F73">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G73">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H73">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
+        <v>17</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B74" t="s">
-        <v>12</v>
-      </c>
       <c r="C74">
         <v>34</v>
       </c>
       <c r="D74">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E74">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F74">
         <v>8</v>
       </c>
       <c r="G74">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="H74">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>17</v>
-      </c>
-      <c r="B75" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C75">
         <v>34</v>
       </c>
       <c r="D75">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E75">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F75">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G75">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H75">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
+        <v>19</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C76">
+        <v>34</v>
+      </c>
+      <c r="D76">
+        <v>6</v>
+      </c>
+      <c r="E76">
         <v>18</v>
       </c>
-      <c r="B76" t="s">
-        <v>17</v>
-      </c>
-      <c r="C76">
-        <v>34</v>
-      </c>
-      <c r="D76">
-        <v>10</v>
-      </c>
-      <c r="E76">
-        <v>17</v>
-      </c>
       <c r="F76">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G76">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H76">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>19</v>
-      </c>
-      <c r="B77" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C77">
         <v>34</v>
       </c>
       <c r="D77">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E77">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F77">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G77">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="H77">
         <v>2015</v>
@@ -2492,25 +2497,25 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>20</v>
-      </c>
-      <c r="B78" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C78">
         <v>34</v>
       </c>
       <c r="D78">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E78">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F78">
         <v>6</v>
       </c>
       <c r="G78">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H78">
         <v>2015</v>
@@ -2518,36 +2523,36 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>1</v>
-      </c>
-      <c r="B79" t="s">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C79">
         <v>34</v>
       </c>
       <c r="D79">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E79">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F79">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G79">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H79">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>2</v>
-      </c>
-      <c r="B80" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C80">
         <v>34</v>
@@ -2556,50 +2561,50 @@
         <v>15</v>
       </c>
       <c r="E80">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F80">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G80">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H80">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>3</v>
-      </c>
-      <c r="B81" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C81">
         <v>34</v>
       </c>
       <c r="D81">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E81">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F81">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G81">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H81">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>4</v>
-      </c>
-      <c r="B82" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C82">
         <v>34</v>
@@ -2608,76 +2613,76 @@
         <v>15</v>
       </c>
       <c r="E82">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F82">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G82">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H82">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>5</v>
-      </c>
-      <c r="B83" t="s">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C83">
         <v>34</v>
       </c>
       <c r="D83">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E83">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F83">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G83">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H83">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
+        <v>8</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84">
+        <v>34</v>
+      </c>
+      <c r="D84">
+        <v>15</v>
+      </c>
+      <c r="E84">
+        <v>13</v>
+      </c>
+      <c r="F84">
         <v>6</v>
       </c>
-      <c r="B84" t="s">
-        <v>26</v>
-      </c>
-      <c r="C84">
-        <v>34</v>
-      </c>
-      <c r="D84">
-        <v>12</v>
-      </c>
-      <c r="E84">
-        <v>6</v>
-      </c>
-      <c r="F84">
-        <v>16</v>
-      </c>
       <c r="G84">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H84">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>7</v>
-      </c>
-      <c r="B85" t="s">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C85">
         <v>34</v>
@@ -2686,128 +2691,128 @@
         <v>14</v>
       </c>
       <c r="E85">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F85">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G85">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H85">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>8</v>
-      </c>
-      <c r="B86" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C86">
         <v>34</v>
       </c>
       <c r="D86">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E86">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F86">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G86">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H86">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>9</v>
-      </c>
-      <c r="B87" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C87">
         <v>34</v>
       </c>
       <c r="D87">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E87">
         <v>12</v>
       </c>
       <c r="F87">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G87">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H87">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>10</v>
-      </c>
-      <c r="B88" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C88">
         <v>34</v>
       </c>
       <c r="D88">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E88">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F88">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G88">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H88">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>11</v>
-      </c>
-      <c r="B89" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C89">
         <v>34</v>
       </c>
       <c r="D89">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E89">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F89">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G89">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H89">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>12</v>
-      </c>
-      <c r="B90" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C90">
         <v>34</v>
@@ -2825,15 +2830,15 @@
         <v>44</v>
       </c>
       <c r="H90">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>13</v>
-      </c>
-      <c r="B91" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C91">
         <v>34</v>
@@ -2851,15 +2856,15 @@
         <v>42</v>
       </c>
       <c r="H91">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>14</v>
-      </c>
-      <c r="B92" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C92">
         <v>34</v>
@@ -2868,50 +2873,50 @@
         <v>11</v>
       </c>
       <c r="E92">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F92">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G92">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H92">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>15</v>
-      </c>
-      <c r="B93" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C93">
         <v>34</v>
       </c>
       <c r="D93">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E93">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F93">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G93">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H93">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>16</v>
-      </c>
-      <c r="B94" t="s">
-        <v>30</v>
+        <v>18</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C94">
         <v>34</v>
@@ -2920,50 +2925,50 @@
         <v>10</v>
       </c>
       <c r="E94">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F94">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G94">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H94">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>17</v>
-      </c>
-      <c r="B95" t="s">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C95">
         <v>34</v>
       </c>
       <c r="D95">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E95">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F95">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G95">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H95">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>18</v>
-      </c>
-      <c r="B96" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C96">
         <v>34</v>
@@ -2972,39 +2977,39 @@
         <v>8</v>
       </c>
       <c r="E96">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F96">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G96">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H96">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>19</v>
-      </c>
-      <c r="B97" t="s">
         <v>1</v>
       </c>
+      <c r="B97" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C97">
         <v>34</v>
       </c>
       <c r="D97">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E97">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F97">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G97">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="H97">
         <v>2016</v>
@@ -3012,25 +3017,25 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>20</v>
-      </c>
-      <c r="B98" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C98">
         <v>34</v>
       </c>
       <c r="D98">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E98">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F98">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G98">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="H98">
         <v>2016</v>
@@ -3038,493 +3043,493 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>1</v>
-      </c>
-      <c r="B99" t="s">
-        <v>21</v>
+        <v>3</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C99">
         <v>34</v>
       </c>
       <c r="D99">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E99">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F99">
         <v>9</v>
       </c>
       <c r="G99">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="H99">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>2</v>
-      </c>
-      <c r="B100" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C100">
         <v>34</v>
       </c>
       <c r="D100">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E100">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F100">
         <v>9</v>
       </c>
       <c r="G100">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H100">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>3</v>
-      </c>
-      <c r="B101" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C101">
         <v>34</v>
       </c>
       <c r="D101">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E101">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F101">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G101">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H101">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>4</v>
-      </c>
-      <c r="B102" t="s">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C102">
         <v>34</v>
       </c>
       <c r="D102">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E102">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F102">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G102">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H102">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>5</v>
-      </c>
-      <c r="B103" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C103">
         <v>34</v>
       </c>
       <c r="D103">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E103">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F103">
         <v>6</v>
       </c>
       <c r="G103">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H103">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>6</v>
-      </c>
-      <c r="B104" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C104">
         <v>34</v>
       </c>
       <c r="D104">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E104">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F104">
         <v>8</v>
       </c>
       <c r="G104">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H104">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>7</v>
-      </c>
-      <c r="B105" t="s">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C105">
         <v>34</v>
       </c>
       <c r="D105">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E105">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F105">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G105">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H105">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>8</v>
-      </c>
-      <c r="B106" t="s">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C106">
         <v>34</v>
       </c>
       <c r="D106">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E106">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F106">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G106">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H106">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>9</v>
-      </c>
-      <c r="B107" t="s">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C107">
         <v>34</v>
       </c>
       <c r="D107">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E107">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F107">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G107">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H107">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>10</v>
-      </c>
-      <c r="B108" t="s">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C108">
         <v>34</v>
       </c>
       <c r="D108">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E108">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F108">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G108">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H108">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>11</v>
-      </c>
-      <c r="B109" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C109">
         <v>34</v>
       </c>
       <c r="D109">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E109">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F109">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G109">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H109">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>12</v>
-      </c>
-      <c r="B110" t="s">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C110">
         <v>34</v>
       </c>
       <c r="D110">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E110">
         <v>14</v>
       </c>
       <c r="F110">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G110">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H110">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>13</v>
-      </c>
-      <c r="B111" t="s">
-        <v>15</v>
+        <v>15</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C111">
         <v>34</v>
       </c>
       <c r="D111">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E111">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F111">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G111">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H111">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>14</v>
-      </c>
-      <c r="B112" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C112">
         <v>34</v>
       </c>
       <c r="D112">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E112">
         <v>15</v>
       </c>
       <c r="F112">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G112">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H112">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>15</v>
-      </c>
-      <c r="B113" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C113">
         <v>34</v>
       </c>
       <c r="D113">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E113">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F113">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G113">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H113">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>16</v>
-      </c>
-      <c r="B114" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C114">
         <v>34</v>
       </c>
       <c r="D114">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E114">
         <v>14</v>
       </c>
       <c r="F114">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G114">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H114">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>17</v>
-      </c>
-      <c r="B115" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C115">
         <v>34</v>
       </c>
       <c r="D115">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E115">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F115">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G115">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H115">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>18</v>
-      </c>
-      <c r="B116" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C116">
         <v>34</v>
       </c>
       <c r="D116">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E116">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F116">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G116">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H116">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>19</v>
-      </c>
-      <c r="B117" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C117">
         <v>34</v>
       </c>
       <c r="D117">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E117">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F117">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G117">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="H117">
         <v>2017</v>
@@ -3532,25 +3537,25 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>20</v>
-      </c>
-      <c r="B118" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C118">
+        <v>34</v>
+      </c>
+      <c r="D118">
         <v>16</v>
       </c>
-      <c r="C118">
-        <v>34</v>
-      </c>
-      <c r="D118">
-        <v>9</v>
-      </c>
       <c r="E118">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F118">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G118">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="H118">
         <v>2017</v>
@@ -3558,25 +3563,25 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>21</v>
-      </c>
-      <c r="B119" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C119">
         <v>34</v>
       </c>
       <c r="D119">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E119">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F119">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G119">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="H119">
         <v>2017</v>
@@ -3584,32 +3589,510 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>22</v>
-      </c>
-      <c r="B120" t="s">
-        <v>26</v>
+        <v>4</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C120">
         <v>34</v>
       </c>
       <c r="D120">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E120">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F120">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G120">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="H120">
         <v>2017</v>
       </c>
     </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>5</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C121">
+        <v>34</v>
+      </c>
+      <c r="D121">
+        <v>16</v>
+      </c>
+      <c r="E121">
+        <v>12</v>
+      </c>
+      <c r="F121">
+        <v>6</v>
+      </c>
+      <c r="G121">
+        <v>54</v>
+      </c>
+      <c r="H121">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>6</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C122">
+        <v>34</v>
+      </c>
+      <c r="D122">
+        <v>15</v>
+      </c>
+      <c r="E122">
+        <v>11</v>
+      </c>
+      <c r="F122">
+        <v>8</v>
+      </c>
+      <c r="G122">
+        <v>53</v>
+      </c>
+      <c r="H122">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>7</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C123">
+        <v>34</v>
+      </c>
+      <c r="D123">
+        <v>14</v>
+      </c>
+      <c r="E123">
+        <v>9</v>
+      </c>
+      <c r="F123">
+        <v>11</v>
+      </c>
+      <c r="G123">
+        <v>53</v>
+      </c>
+      <c r="H123">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>8</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C124">
+        <v>34</v>
+      </c>
+      <c r="D124">
+        <v>15</v>
+      </c>
+      <c r="E124">
+        <v>12</v>
+      </c>
+      <c r="F124">
+        <v>7</v>
+      </c>
+      <c r="G124">
+        <v>52</v>
+      </c>
+      <c r="H124">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>9</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>34</v>
+      </c>
+      <c r="D125">
+        <v>14</v>
+      </c>
+      <c r="E125">
+        <v>12</v>
+      </c>
+      <c r="F125">
+        <v>8</v>
+      </c>
+      <c r="G125">
+        <v>50</v>
+      </c>
+      <c r="H125">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>10</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126">
+        <v>34</v>
+      </c>
+      <c r="D126">
+        <v>13</v>
+      </c>
+      <c r="E126">
+        <v>10</v>
+      </c>
+      <c r="F126">
+        <v>11</v>
+      </c>
+      <c r="G126">
+        <v>50</v>
+      </c>
+      <c r="H126">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>11</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C127">
+        <v>34</v>
+      </c>
+      <c r="D127">
+        <v>12</v>
+      </c>
+      <c r="E127">
+        <v>9</v>
+      </c>
+      <c r="F127">
+        <v>13</v>
+      </c>
+      <c r="G127">
+        <v>49</v>
+      </c>
+      <c r="H127">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>12</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C128">
+        <v>34</v>
+      </c>
+      <c r="D128">
+        <v>13</v>
+      </c>
+      <c r="E128">
+        <v>14</v>
+      </c>
+      <c r="F128">
+        <v>7</v>
+      </c>
+      <c r="G128">
+        <v>46</v>
+      </c>
+      <c r="H128">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>13</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129">
+        <v>34</v>
+      </c>
+      <c r="D129">
+        <v>11</v>
+      </c>
+      <c r="E129">
+        <v>10</v>
+      </c>
+      <c r="F129">
+        <v>13</v>
+      </c>
+      <c r="G129">
+        <v>46</v>
+      </c>
+      <c r="H129">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>14</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130">
+        <v>34</v>
+      </c>
+      <c r="D130">
+        <v>13</v>
+      </c>
+      <c r="E130">
+        <v>15</v>
+      </c>
+      <c r="F130">
+        <v>6</v>
+      </c>
+      <c r="G130">
+        <v>45</v>
+      </c>
+      <c r="H130">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>15</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C131">
+        <v>34</v>
+      </c>
+      <c r="D131">
+        <v>13</v>
+      </c>
+      <c r="E131">
+        <v>15</v>
+      </c>
+      <c r="F131">
+        <v>6</v>
+      </c>
+      <c r="G131">
+        <v>45</v>
+      </c>
+      <c r="H131">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>16</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C132">
+        <v>34</v>
+      </c>
+      <c r="D132">
+        <v>11</v>
+      </c>
+      <c r="E132">
+        <v>14</v>
+      </c>
+      <c r="F132">
+        <v>9</v>
+      </c>
+      <c r="G132">
+        <v>42</v>
+      </c>
+      <c r="H132">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>17</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C133">
+        <v>34</v>
+      </c>
+      <c r="D133">
+        <v>11</v>
+      </c>
+      <c r="E133">
+        <v>17</v>
+      </c>
+      <c r="F133">
+        <v>6</v>
+      </c>
+      <c r="G133">
+        <v>39</v>
+      </c>
+      <c r="H133">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>18</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C134">
+        <v>34</v>
+      </c>
+      <c r="D134">
+        <v>10</v>
+      </c>
+      <c r="E134">
+        <v>15</v>
+      </c>
+      <c r="F134">
+        <v>9</v>
+      </c>
+      <c r="G134">
+        <v>39</v>
+      </c>
+      <c r="H134">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>19</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C135">
+        <v>34</v>
+      </c>
+      <c r="D135">
+        <v>10</v>
+      </c>
+      <c r="E135">
+        <v>18</v>
+      </c>
+      <c r="F135">
+        <v>6</v>
+      </c>
+      <c r="G135">
+        <v>36</v>
+      </c>
+      <c r="H135">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>20</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C136">
+        <v>34</v>
+      </c>
+      <c r="D136">
+        <v>9</v>
+      </c>
+      <c r="E136">
+        <v>19</v>
+      </c>
+      <c r="F136">
+        <v>6</v>
+      </c>
+      <c r="G136">
+        <v>33</v>
+      </c>
+      <c r="H136">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>21</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C137">
+        <v>34</v>
+      </c>
+      <c r="D137">
+        <v>9</v>
+      </c>
+      <c r="E137">
+        <v>20</v>
+      </c>
+      <c r="F137">
+        <v>5</v>
+      </c>
+      <c r="G137">
+        <v>32</v>
+      </c>
+      <c r="H137">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>22</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C138">
+        <v>34</v>
+      </c>
+      <c r="D138">
+        <v>8</v>
+      </c>
+      <c r="E138">
+        <v>18</v>
+      </c>
+      <c r="F138">
+        <v>8</v>
+      </c>
+      <c r="G138">
+        <v>32</v>
+      </c>
+      <c r="H138">
+        <v>2017</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{DD1629E0-43CA-4C40-A6B9-C484ED9C006D}">
+    <sortState ref="A2:H138">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A2:H138">
+    <sortCondition ref="H2:H138"/>
+    <sortCondition ref="A2:A138"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>